<commit_message>
Committed for POI implementation.
</commit_message>
<xml_diff>
--- a/emp-perf-service/resources/timesheet.xlsx
+++ b/emp-perf-service/resources/timesheet.xlsx
@@ -27,30 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Mrinmay</t>
   </si>
   <si>
     <t>23.10.2018</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Swipe In</t>
-  </si>
-  <si>
-    <t>Swipe Out</t>
-  </si>
-  <si>
-    <t>Minute</t>
-  </si>
-  <si>
-    <t>Minute Code</t>
   </si>
 </sst>
 </file>
@@ -412,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,77 +412,57 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E1" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="F1" s="3">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+      <c r="D2" s="2">
         <v>0.375</v>
       </c>
-      <c r="F2" s="3">
-        <v>60</v>
+      <c r="E2" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F2" s="1">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="1">
-        <v>123</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="F3" s="1">
-        <v>120</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="3"/>
-      <c r="D4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="C4" s="1">
+        <v>123</v>
+      </c>
+      <c r="D4" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="1">
-        <v>123</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="E4" s="2">
         <v>0.25</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F4" s="1">
         <v>240</v>
       </c>
     </row>

</xml_diff>